<commit_message>
Finalização do Manual e alterações no Burndown
</commit_message>
<xml_diff>
--- a/Burndown/Grafico Burndown.xlsx
+++ b/Burndown/Grafico Burndown.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\PIM\Burndown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327A6FAD-60D9-4C3D-9A74-462FC1AD76B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80C8A5B-5C0D-4614-BFE2-349B2C412F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D1D58205-FE73-4A1A-9CC0-804F53F71D92}"/>
   </bookViews>
@@ -492,31 +492,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -588,31 +588,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.5</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.5</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1713,7 +1713,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0891ED6A-1E66-4016-A54C-BFB5A0A4EA05}">
-  <dimension ref="B1:E18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1753,10 +1753,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="11">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D5" s="11">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E5" s="12">
         <v>5.5</v>
@@ -1767,10 +1767,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1">
-        <v>34.5</v>
+        <v>38.5</v>
       </c>
       <c r="E6" s="3">
         <v>4.4000000000000004</v>
@@ -1781,10 +1781,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
@@ -1795,10 +1795,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E8" s="3">
         <v>3</v>
@@ -1809,10 +1809,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E9" s="3">
         <v>4.5</v>
@@ -1823,10 +1823,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1">
-        <v>16.5</v>
+        <v>20.5</v>
       </c>
       <c r="E10" s="3">
         <v>5</v>
@@ -1837,10 +1837,10 @@
         <v>5</v>
       </c>
       <c r="C11" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1">
-        <v>11.5</v>
+        <v>15.5</v>
       </c>
       <c r="E11" s="3">
         <v>5.5</v>
@@ -1851,10 +1851,10 @@
         <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E12" s="3">
         <v>6</v>
@@ -1865,10 +1865,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D13" s="5">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="E13" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
Adição da Sprint 9 e Alterações no Burndown
</commit_message>
<xml_diff>
--- a/Burndown/Grafico Burndown.xlsx
+++ b/Burndown/Grafico Burndown.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\PIM\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80C8A5B-5C0D-4614-BFE2-349B2C412F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E71B753-B5E2-48EE-8FC7-593589EA66DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D1D58205-FE73-4A1A-9CC0-804F53F71D92}"/>
   </bookViews>
   <sheets>
-    <sheet name="Burndown" sheetId="1" r:id="rId1"/>
+    <sheet name="Burndown" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,26 +60,26 @@
     <t>Sprint 8</t>
   </si>
   <si>
-    <t>Base Line</t>
-  </si>
-  <si>
     <t>Horas Trabalhadas</t>
   </si>
   <si>
-    <t>Resultado em Horas</t>
+    <t>Sprint</t>
   </si>
   <si>
-    <t>Sprint 0</t>
+    <t>Sprint 9</t>
   </si>
   <si>
-    <t>Sprint</t>
+    <t>Horas Restantes</t>
+  </si>
+  <si>
+    <t>Horas Acumuladas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,12 +95,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -134,10 +128,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -152,10 +146,55 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -167,40 +206,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -212,43 +221,13 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -257,10 +236,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -269,25 +248,49 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -302,15 +305,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -322,22 +322,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -392,7 +398,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
-              <a:t>Gráfico Burndown</a:t>
+              <a:t>Burndown</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -435,9 +441,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Base Line</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -456,31 +459,31 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>Sprint 0</c:v>
+                  <c:v>Sprint 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
+                  <c:v>Sprint 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
+                  <c:v>Sprint 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
+                  <c:v>Sprint 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
+                  <c:v>Sprint 5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
+                  <c:v>Sprint 6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Sprint 6</c:v>
+                  <c:v>Sprint 7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Sprint 7</c:v>
+                  <c:v>Sprint 8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Sprint 8</c:v>
+                  <c:v>Sprint 9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -492,31 +495,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -524,16 +527,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1558-4232-BE27-314604DB4CDA}"/>
+              <c16:uniqueId val="{00000000-22EF-4EFB-BD4C-0A85798F3BF2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Horas Trabalhadas</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -552,67 +552,67 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>Sprint 0</c:v>
+                  <c:v>Sprint 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sprint 1</c:v>
+                  <c:v>Sprint 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Sprint 2</c:v>
+                  <c:v>Sprint 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Sprint 3</c:v>
+                  <c:v>Sprint 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Sprint 4</c:v>
+                  <c:v>Sprint 5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
+                  <c:v>Sprint 6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Sprint 6</c:v>
+                  <c:v>Sprint 7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Sprint 7</c:v>
+                  <c:v>Sprint 8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Sprint 8</c:v>
+                  <c:v>Sprint 9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$D$5:$D$13</c:f>
+              <c:f>Burndown!$E$5:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.5</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>46.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.5</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.5</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -620,7 +620,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1558-4232-BE27-314604DB4CDA}"/>
+              <c16:uniqueId val="{00000001-22EF-4EFB-BD4C-0A85798F3BF2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -633,11 +633,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1578392848"/>
-        <c:axId val="1578391408"/>
+        <c:axId val="235286607"/>
+        <c:axId val="235290447"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1578392848"/>
+        <c:axId val="235286607"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +680,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1578391408"/>
+        <c:crossAx val="235290447"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -688,7 +688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1578391408"/>
+        <c:axId val="235290447"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,7 +739,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1578392848"/>
+        <c:crossAx val="235286607"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1380,22 +1380,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>404812</xdr:colOff>
+      <xdr:colOff>442912</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>195262</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:colOff>233362</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Gráfico 10">
+        <xdr:cNvPr id="5" name="Gráfico 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C0A7E85-28E9-CB81-0E9D-000E04ED6AC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05A7C225-38B0-EAA0-CF4D-1E03D94FBF1F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1712,175 +1712,178 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0891ED6A-1E66-4016-A54C-BFB5A0A4EA05}">
-  <dimension ref="A1:N18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88370CA0-5665-475C-A66B-1B486B025687}">
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="12" width="9.140625" customWidth="1"/>
     <col min="13" max="13" width="4.28515625" customWidth="1"/>
     <col min="14" max="14" width="2.7109375" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" hidden="1"/>
+    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="2:5" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+    </row>
+    <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12">
+        <v>63</v>
+      </c>
+      <c r="D5" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10">
+        <v>56</v>
+      </c>
+      <c r="D6" s="1">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="10">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="10">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1">
         <v>8</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E9" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="10">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1">
         <v>9</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>10</v>
+      <c r="E10" s="2">
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="11">
-        <v>45</v>
-      </c>
-      <c r="D5" s="11">
-        <v>45</v>
-      </c>
-      <c r="E5" s="12">
-        <v>5.5</v>
+    <row r="11" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="10">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2">
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>40</v>
-      </c>
-      <c r="D6" s="1">
-        <v>38.5</v>
-      </c>
-      <c r="E6" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1">
-        <v>34</v>
-      </c>
-      <c r="E7" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1">
-        <v>28</v>
-      </c>
-      <c r="E8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1">
-        <v>25</v>
-      </c>
-      <c r="E9" s="3">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1">
-        <v>20.5</v>
-      </c>
-      <c r="E10" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1">
-        <v>15.5</v>
-      </c>
-      <c r="E11" s="3">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1">
-        <v>10</v>
+    <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="10">
+        <v>14</v>
       </c>
       <c r="D12" s="1">
-        <v>10</v>
-      </c>
-      <c r="E12" s="3">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E12" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="11">
         <v>7</v>
       </c>
-      <c r="C13" s="5">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5">
-        <v>8.5</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
+      <c r="D13" s="13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25"/>
-    <row r="17" x14ac:dyDescent="0.25"/>
-    <row r="18" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:5" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>